<commit_message>
Correções aos ficheiros existentes, colocação da blueprint final
</commit_message>
<xml_diff>
--- a/back-end/BE Services data.xlsx
+++ b/back-end/BE Services data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\back-end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guicu\Documents\Universidade\Mestrado\2Semestre\Aplicações na web\aw-project\back-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DAAB45-7EB8-4AEA-8E36-96D14DC39D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB39F2B-DB3C-446B-990B-0D337E524126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{7339BE56-F3CD-4EA2-BB4E-FEE8F77C3A35}"/>
+    <workbookView xWindow="22932" yWindow="-84" windowWidth="23256" windowHeight="12456" xr2:uid="{7339BE56-F3CD-4EA2-BB4E-FEE8F77C3A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>BE Service</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>feedback/{meatID}</t>
-  </si>
-  <si>
-    <t>saved/{userID}/{productID}</t>
   </si>
   <si>
     <t>saved/{userID}</t>
@@ -130,11 +127,6 @@
   <si>
     <t>MarketList{
  [Market]
- }</t>
-  </si>
-  <si>
-    <t>Categories: {
- Enum: [Chicken, Beef, Pork, Lamb, Goat, Exotic Meats],
  }</t>
   </si>
   <si>
@@ -147,12 +139,6 @@
  "name": string,
  "location": string,
  "categories":[Categories]
- }</t>
-  </si>
-  <si>
-    <t>News: {
- "image": string($uri),
- "text": string
  }</t>
   </si>
   <si>
@@ -172,11 +158,6 @@
     <t>Feedback: {
  "username": string,
  "star_review": integer
- }</t>
-  </si>
-  <si>
-    <t>Saved: {
- [Product]
  }</t>
   </si>
   <si>
@@ -193,6 +174,29 @@
  "analytics": boolean,
  "auto_update": boolean,
  "data_storage":Enum: [local,cloud]
+ }</t>
+  </si>
+  <si>
+    <t>News: {
+ "id": number,
+ "image": string($uri),
+ "title": string,
+ "text": string,
+ "date": string
+ }</t>
+  </si>
+  <si>
+    <t>Categories: {
+ Enum: [Chicken, Beef, Pork, Lamb, Turkey, Goat, Ready to cook, Exotic Meats],
+ }</t>
+  </si>
+  <si>
+    <t>Product: {
+ "id": number,
+ "name": string,
+ "price_per_kilo": number,
+ "location": string,                        "details": string,
+ "full_details": string
  }</t>
   </si>
 </sst>
@@ -249,13 +253,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -275,7 +279,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -573,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40E9603-68F7-4D15-97A9-F1A4E612FDFE}">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,228 +608,228 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>26</v>
+    <row r="4" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>24</v>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>25</v>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
+    <row r="18" spans="2:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>